<commit_message>
Return max count for Json entity.
</commit_message>
<xml_diff>
--- a/testExcel.xlsx
+++ b/testExcel.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Documents\GitHub\ReadExcelWithJS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F5EC95E-9625-4F85-8C4A-2A1FAA303B36}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8913E2EB-06BA-4381-9E1F-2CC436482597}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3255" yWindow="945" windowWidth="21600" windowHeight="11385" xr2:uid="{CDD65AAA-F0F7-4A44-BA06-FFA93F39CF83}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{CDD65AAA-F0F7-4A44-BA06-FFA93F39CF83}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -404,7 +404,7 @@
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -443,10 +443,10 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B5" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>